<commit_message>
working on excel for master data
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -339,23 +339,88 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>shubham</v>
+        <v>UserName</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Password</v>
+      </c>
+      <c r="C1" t="str">
+        <v>UserRole</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>MobileNo</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>dev_1</v>
+        <v>shubham</v>
+      </c>
+      <c r="B2" t="str">
+        <v>dev_123</v>
+      </c>
+      <c r="C2" t="str">
+        <v>developers</v>
+      </c>
+      <c r="D2" t="str">
+        <v>shubham@blog.com</v>
+      </c>
+      <c r="E2">
+        <v>1122334455</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>gaurav</v>
       </c>
+      <c r="B3" t="str">
+        <v>check_1233</v>
+      </c>
+      <c r="C3" t="str">
+        <v>tester</v>
+      </c>
+      <c r="D3" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E3">
+        <v>9988273</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
         <v>gaurav</v>
       </c>
+      <c r="B4" t="str">
+        <v>check_1233</v>
+      </c>
+      <c r="C4" t="str">
+        <v>tester</v>
+      </c>
+      <c r="D4" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E4">
+        <v>9988273</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>dev_1</v>
+      </c>
+      <c r="B5" t="str">
+        <v>check_1233</v>
+      </c>
+      <c r="C5" t="str">
+        <v>tester</v>
+      </c>
+      <c r="D5" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E5">
+        <v>9988273</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>